<commit_message>
Edit total for December 14, 2021
</commit_message>
<xml_diff>
--- a/applications.xlsx
+++ b/applications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57419\Documents\applications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AD9D75-97F5-4725-8DC7-4B82FB053123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BF06DE-B90D-40CE-9C64-CC4CEE80625C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48525" yWindow="1455" windowWidth="8100" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2478" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="1131">
   <si>
     <t>Total</t>
   </si>
@@ -3786,8 +3786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3958,8 +3958,8 @@
     </row>
     <row r="2" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <f xml:space="preserve"> COUNTA(C2:AAD100)</f>
-        <v>1188</v>
+        <f xml:space="preserve"> COUNTA(B2:AAD100)</f>
+        <v>1238</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1087</v>

</xml_diff>